<commit_message>
sumproduct() working on example.xlsx
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" activeTab="1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -685,18 +685,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1">
-        <f>SUM(Sheet1!A1:A18)</f>
-        <v>187</v>
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <f>SUMPRODUCT(A1:A3*B1:B3*(C1:C3&lt;9))</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>